<commit_message>
2nd commit after ques 2
</commit_message>
<xml_diff>
--- a/TtAssignment.xlsx
+++ b/TtAssignment.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Question_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Question_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="279">
   <si>
     <t>Project Name</t>
   </si>
@@ -606,7 +607,7 @@
 </t>
   </si>
   <si>
-    <t>Update Button should not be clicked and mouse shoul be cross marked</t>
+    <t>Update Button should not be clicked and mouse should be cross marked</t>
   </si>
   <si>
     <t xml:space="preserve">Update button is clicked and "screen updated-screen_name" pop up displayed
@@ -626,9 +627,6 @@
   </si>
   <si>
     <t>1.user should be on screener page after creating a new screen</t>
-  </si>
-  <si>
-    <t>Update Button should not be clicked and mouse should be cross marked</t>
   </si>
   <si>
     <t>Tc_UpdateScreen_003</t>
@@ -865,25 +863,202 @@
     <t>1.First click PE Ratiowill be sorted from  higher to lower
 2.Second click PE Ratio will be sorted to lower to higher</t>
   </si>
+  <si>
+    <t>serial_no</t>
+  </si>
+  <si>
+    <t>Defect_Id</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Reproducible (yes/no)</t>
+  </si>
+  <si>
+    <t>Steps to reproduce</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reported By </t>
+  </si>
+  <si>
+    <t>Reported Date</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>DEF_001</t>
+  </si>
+  <si>
+    <t>User is abel to create watchlist with same name</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.use
+r should be logged into Tickertape and should be on Homepage
+2.Click on watchList From navbar
+3.Click on Create Equity Watchlist on left pane
+4.Create one watchlist named "Equity watchlist"
+5.create another watchlist with same name
+</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26-01-2022</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to add a stock from floating navbar or try to create watchlist with same name from watchlist section
+</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>DEF_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No option to add stock in Busket when trying to add directly from busket
+</t>
+  </si>
+  <si>
+    <t>1.User should be logged into Tickertape and should be on Homepage
+2.click on Basket from navbar
+3.click on search Stocks(no stocks is added to busket already)
+4.search for stock (Reliance Industries)
+5.Mouse over to any stock</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There should be an option to add Stock directly feom searchbar as we have already one for watchlist
+</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>DEF_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About Us and Contact Us page is redirecting to the same page
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.User should be logged into Tickertape and should be on Homepage   
+2.click on About Us at Bottom of the page
+3.Navigate to Homepage
+4.click on Contack Us </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can change the approach like smallcase have
+</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>DEF_004</t>
+  </si>
+  <si>
+    <t>Sorting By Name On Screener Page</t>
+  </si>
+  <si>
+    <t>1.user is logged in to Tickertape and on screener page
+2.click on Name↓ on the right pane to sort [Z-A,9-0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not sorted Properly from [z-a] "shipping corporation of india is coming"
+</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>DEF_005</t>
+  </si>
+  <si>
+    <t>User is abel to Update without changing name or description</t>
+  </si>
+  <si>
+    <t>1.user should be on manage screens page
+2.user should open one already existing screen from navbar
+3.click on pencil symbol beside load button
+4.do not change any existing data from name field and description field
+5.click on update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.After Clicking on update pop up"Screen updated - New Screen" is coming
+2.update button should be greyd out till make any changes
+</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>DEF_006</t>
+  </si>
+  <si>
+    <t>User is abel to click on update before making any changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.user should be on screener page after creating a new screen
+or selection on already existing screen
+3..mouse hover to update button
+4.click on update button
+</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -900,7 +1075,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -910,14 +1091,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -938,6 +1120,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -948,14 +1138,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -985,6 +1167,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -992,31 +1182,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1035,6 +1202,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="39">
     <fill>
@@ -1045,6 +1220,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.25"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1052,12 +1233,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,31 +1256,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1123,6 +1286,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1135,13 +1340,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1153,49 +1364,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1213,31 +1394,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1249,7 +1406,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1261,17 +1418,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1286,50 +1476,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1367,8 +1513,52 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1377,162 +1567,192 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="10" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="10" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
@@ -1550,46 +1770,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1598,25 +1797,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1941,9 +2131,9 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1963,221 +2153,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
     </row>
     <row r="5" ht="17" customHeight="1" spans="1:20">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
     </row>
     <row r="7" ht="21" customHeight="1" spans="1:20">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A8" s="1" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+    </row>
+    <row r="8" s="13" customFormat="1" ht="23" customHeight="1" spans="1:13">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2185,22 +2375,22 @@
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J9" t="s">
@@ -2209,7 +2399,7 @@
       <c r="K9" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="27">
+      <c r="L9" s="30">
         <v>44586</v>
       </c>
       <c r="M9" t="s">
@@ -2220,22 +2410,22 @@
       <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J10" t="s">
@@ -2244,7 +2434,7 @@
       <c r="K10" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="30">
         <v>44586</v>
       </c>
       <c r="M10" t="s">
@@ -2255,22 +2445,22 @@
       <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="5" t="s">
         <v>44</v>
       </c>
       <c r="J11" t="s">
@@ -2279,7 +2469,7 @@
       <c r="K11" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="27">
+      <c r="L11" s="30">
         <v>44586</v>
       </c>
       <c r="M11" t="s">
@@ -2290,25 +2480,25 @@
       <c r="A12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="5" t="s">
         <v>51</v>
       </c>
       <c r="J12" t="s">
@@ -2317,7 +2507,7 @@
       <c r="K12" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="27">
+      <c r="L12" s="30">
         <v>44586</v>
       </c>
       <c r="M12" t="s">
@@ -2328,25 +2518,25 @@
       <c r="A13" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="5" t="s">
         <v>51</v>
       </c>
       <c r="J13" t="s">
@@ -2355,7 +2545,7 @@
       <c r="K13" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="27">
+      <c r="L13" s="30">
         <v>44586</v>
       </c>
       <c r="M13" t="s">
@@ -2366,25 +2556,25 @@
       <c r="A14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="5" t="s">
         <v>51</v>
       </c>
       <c r="J14" t="s">
@@ -2393,7 +2583,7 @@
       <c r="K14" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="27">
+      <c r="L14" s="30">
         <v>44586</v>
       </c>
       <c r="M14" t="s">
@@ -2404,25 +2594,25 @@
       <c r="A15" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="5" t="s">
         <v>65</v>
       </c>
       <c r="J15" t="s">
@@ -2431,7 +2621,7 @@
       <c r="K15" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="27">
+      <c r="L15" s="30">
         <v>44586</v>
       </c>
       <c r="M15" t="s">
@@ -2442,32 +2632,32 @@
       <c r="A16" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="10"/>
+      <c r="H16" s="5"/>
       <c r="J16" t="s">
         <v>32</v>
       </c>
       <c r="K16" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="30">
         <v>44586</v>
       </c>
       <c r="M16" t="s">
@@ -2478,25 +2668,25 @@
       <c r="A17" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C17" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="5" t="s">
         <v>76</v>
       </c>
       <c r="J17" t="s">
@@ -2505,47 +2695,47 @@
       <c r="K17" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="27">
+      <c r="L17" s="30">
         <v>44586</v>
       </c>
       <c r="M17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" s="2" customFormat="1" ht="40" customHeight="1" spans="1:13">
-      <c r="A18" s="6" t="s">
+    <row r="18" s="14" customFormat="1" ht="40" customHeight="1" spans="1:13">
+      <c r="A18" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
     </row>
     <row r="19" ht="90" spans="1:13">
       <c r="A19" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="5" t="s">
         <v>83</v>
       </c>
       <c r="J19" t="s">
@@ -2554,7 +2744,7 @@
       <c r="K19" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="27">
+      <c r="L19" s="30">
         <v>44586</v>
       </c>
       <c r="M19" t="s">
@@ -2565,22 +2755,22 @@
       <c r="A20" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F20" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="5" t="s">
         <v>89</v>
       </c>
       <c r="J20" t="s">
@@ -2589,7 +2779,7 @@
       <c r="K20" t="s">
         <v>7</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="30">
         <v>44586</v>
       </c>
       <c r="M20" t="s">
@@ -2600,22 +2790,22 @@
       <c r="A21" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="5" t="s">
         <v>94</v>
       </c>
       <c r="J21" t="s">
@@ -2624,7 +2814,7 @@
       <c r="K21" t="s">
         <v>7</v>
       </c>
-      <c r="L21" s="27">
+      <c r="L21" s="30">
         <v>44586</v>
       </c>
       <c r="M21" t="s">
@@ -2635,22 +2825,22 @@
       <c r="A22" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="5" t="s">
         <v>99</v>
       </c>
       <c r="J22" t="s">
@@ -2659,7 +2849,7 @@
       <c r="K22" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="27">
+      <c r="L22" s="30">
         <v>44597</v>
       </c>
       <c r="M22" t="s">
@@ -2670,19 +2860,19 @@
       <c r="A23" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C23" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="5" t="s">
         <v>104</v>
       </c>
       <c r="J23" t="s">
@@ -2691,7 +2881,7 @@
       <c r="K23" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="27">
+      <c r="L23" s="30">
         <v>44586</v>
       </c>
       <c r="M23" t="s">
@@ -2699,39 +2889,39 @@
       </c>
     </row>
     <row r="24" ht="36" customHeight="1" spans="1:13">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
     </row>
     <row r="25" ht="60" spans="1:13">
       <c r="A25" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="5" t="s">
         <v>111</v>
       </c>
       <c r="J25" t="s">
@@ -2740,7 +2930,7 @@
       <c r="K25" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="27">
+      <c r="L25" s="30">
         <v>44586</v>
       </c>
       <c r="M25" t="s">
@@ -2751,19 +2941,19 @@
       <c r="A26" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G26" s="5" t="s">
         <v>116</v>
       </c>
       <c r="J26" t="s">
@@ -2772,7 +2962,7 @@
       <c r="K26" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="27">
+      <c r="L26" s="30">
         <v>44586</v>
       </c>
       <c r="M26" t="s">
@@ -2783,19 +2973,19 @@
       <c r="A27" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="5" t="s">
         <v>111</v>
       </c>
       <c r="J27" t="s">
@@ -2804,7 +2994,7 @@
       <c r="K27" t="s">
         <v>7</v>
       </c>
-      <c r="L27" s="27">
+      <c r="L27" s="30">
         <v>44586</v>
       </c>
       <c r="M27" t="s">
@@ -2815,19 +3005,19 @@
       <c r="A28" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="5" t="s">
         <v>116</v>
       </c>
       <c r="J28" t="s">
@@ -2836,7 +3026,7 @@
       <c r="K28" t="s">
         <v>7</v>
       </c>
-      <c r="L28" s="27">
+      <c r="L28" s="30">
         <v>44586</v>
       </c>
       <c r="M28" t="s">
@@ -2844,39 +3034,39 @@
       </c>
     </row>
     <row r="29" ht="37" customHeight="1" spans="1:13">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
     </row>
     <row r="30" ht="75" spans="1:13">
       <c r="A30" t="s">
         <v>125</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="5" t="s">
         <v>129</v>
       </c>
       <c r="J30" t="s">
@@ -2885,7 +3075,7 @@
       <c r="K30" t="s">
         <v>7</v>
       </c>
-      <c r="L30" s="27">
+      <c r="L30" s="30">
         <v>44586</v>
       </c>
       <c r="M30" t="s">
@@ -2896,19 +3086,19 @@
       <c r="A31" t="s">
         <v>130</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="5" t="s">
         <v>133</v>
       </c>
       <c r="J31" t="s">
@@ -2917,7 +3107,7 @@
       <c r="K31" t="s">
         <v>7</v>
       </c>
-      <c r="L31" s="27">
+      <c r="L31" s="30">
         <v>44586</v>
       </c>
       <c r="M31" t="s">
@@ -2928,19 +3118,19 @@
       <c r="A32" t="s">
         <v>134</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C32" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="5" t="s">
         <v>138</v>
       </c>
       <c r="J32" t="s">
@@ -2949,7 +3139,7 @@
       <c r="K32" t="s">
         <v>7</v>
       </c>
-      <c r="L32" s="27">
+      <c r="L32" s="30">
         <v>44586</v>
       </c>
       <c r="M32" t="s">
@@ -2960,22 +3150,22 @@
       <c r="A33" t="s">
         <v>139</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C33" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="5" t="s">
         <v>141</v>
       </c>
       <c r="F33" t="s">
         <v>142</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="5" t="s">
         <v>138</v>
       </c>
       <c r="J33" t="s">
@@ -2984,7 +3174,7 @@
       <c r="K33" t="s">
         <v>7</v>
       </c>
-      <c r="L33" s="27">
+      <c r="L33" s="30">
         <v>44586</v>
       </c>
       <c r="M33" t="s">
@@ -2995,22 +3185,22 @@
       <c r="A34" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="5" t="s">
         <v>145</v>
       </c>
       <c r="F34" t="s">
         <v>142</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G34" s="5" t="s">
         <v>146</v>
       </c>
       <c r="J34" t="s">
@@ -3019,7 +3209,7 @@
       <c r="K34" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="27">
+      <c r="L34" s="30">
         <v>44586</v>
       </c>
       <c r="M34" t="s">
@@ -3030,22 +3220,22 @@
       <c r="A35" t="s">
         <v>147</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="5" t="s">
         <v>149</v>
       </c>
       <c r="F35" t="s">
         <v>142</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G35" s="5" t="s">
         <v>146</v>
       </c>
       <c r="J35" t="s">
@@ -3054,7 +3244,7 @@
       <c r="K35" t="s">
         <v>7</v>
       </c>
-      <c r="L35" s="27">
+      <c r="L35" s="30">
         <v>44586</v>
       </c>
       <c r="M35" t="s">
@@ -3065,22 +3255,22 @@
       <c r="A36" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="5" t="s">
         <v>153</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G36" s="5" t="s">
         <v>155</v>
       </c>
       <c r="J36" t="s">
@@ -3089,7 +3279,7 @@
       <c r="K36" t="s">
         <v>7</v>
       </c>
-      <c r="L36" s="27">
+      <c r="L36" s="30">
         <v>44586</v>
       </c>
       <c r="M36" t="s">
@@ -3097,75 +3287,75 @@
       </c>
     </row>
     <row r="37" ht="27" customHeight="1" spans="1:13">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-    </row>
-    <row r="38" s="3" customFormat="1" ht="90" spans="1:13">
-      <c r="A38" s="13" t="s">
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+    </row>
+    <row r="38" s="15" customFormat="1" ht="90" spans="1:13">
+      <c r="A38" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G38" s="16" t="s">
+      <c r="G38" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="I38" s="16" t="s">
+      <c r="I38" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J38" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="K38" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="L38" s="29">
+      <c r="K38" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L38" s="31">
         <v>44586</v>
       </c>
-      <c r="M38" s="23" t="s">
+      <c r="M38" s="28" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="39" ht="60" spans="1:13">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G39" s="20" t="s">
-        <v>169</v>
+      <c r="G39" s="26" t="s">
+        <v>162</v>
       </c>
       <c r="J39" t="s">
         <v>32</v>
@@ -3173,7 +3363,7 @@
       <c r="K39" t="s">
         <v>7</v>
       </c>
-      <c r="L39" s="27">
+      <c r="L39" s="30">
         <v>44586</v>
       </c>
       <c r="M39" t="s">
@@ -3181,23 +3371,23 @@
       </c>
     </row>
     <row r="40" ht="75" spans="1:13">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C40" s="12" t="s">
+      <c r="D40" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="E40" s="12" t="s">
+      <c r="G40" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>173</v>
       </c>
       <c r="J40" t="s">
         <v>32</v>
@@ -3205,398 +3395,398 @@
       <c r="K40" t="s">
         <v>7</v>
       </c>
-      <c r="L40" s="27">
+      <c r="L40" s="30">
         <v>44586</v>
       </c>
       <c r="M40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" s="4" customFormat="1" ht="90" spans="1:13">
-      <c r="A41" s="13" t="s">
+    <row r="41" s="16" customFormat="1" ht="90" spans="1:13">
+      <c r="A41" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C41" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="D41" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="I41" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="K41" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L41" s="32">
+        <v>44586</v>
+      </c>
+      <c r="M41" s="28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" s="17" customFormat="1" ht="75" spans="1:14">
+      <c r="A42" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B42" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C42" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="D41" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="G41" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="I41" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L41" s="30">
+      <c r="E42" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F42" s="19"/>
+      <c r="G42" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L42" s="33">
         <v>44586</v>
       </c>
-      <c r="M41" s="23" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" s="5" customFormat="1" ht="75" spans="1:14">
-      <c r="A42" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="D42" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="24" t="s">
+      <c r="M42" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N42" s="19"/>
+    </row>
+    <row r="43" s="18" customFormat="1" ht="37" customHeight="1" spans="1:1">
+      <c r="A43" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L42" s="31">
-        <v>44586</v>
-      </c>
-      <c r="M42" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="N42" s="25"/>
-    </row>
-    <row r="43" s="6" customFormat="1" ht="37" customHeight="1" spans="1:1">
-      <c r="A43" s="6" t="s">
+    </row>
+    <row r="44" ht="60" spans="1:13">
+      <c r="A44" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="25" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="44" ht="60" spans="1:13">
-      <c r="A44" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B44" s="18" t="s">
+      <c r="C44" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="D44" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="E44" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="F44" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="G44" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>190</v>
       </c>
       <c r="J44" t="s">
         <v>32</v>
       </c>
-      <c r="K44" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L44" s="31">
+      <c r="K44" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L44" s="33">
         <v>44586</v>
       </c>
-      <c r="M44" s="25" t="s">
+      <c r="M44" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="45" ht="165" spans="1:13">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="B45" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C45" s="12" t="s">
+      <c r="B45" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="E45" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="F45" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="G45" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>195</v>
       </c>
       <c r="J45" t="s">
         <v>32</v>
       </c>
-      <c r="K45" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L45" s="31">
+      <c r="K45" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L45" s="33">
         <v>44586</v>
       </c>
-      <c r="M45" s="25" t="s">
+      <c r="M45" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="46" ht="60" spans="1:13">
-      <c r="A46" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C46" s="12" t="s">
+      <c r="A46" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E46" s="12" t="s">
+      <c r="F46" t="s">
         <v>197</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>199</v>
       </c>
       <c r="J46" t="s">
         <v>32</v>
       </c>
-      <c r="K46" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L46" s="31">
+      <c r="K46" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L46" s="33">
         <v>44586</v>
       </c>
-      <c r="M46" s="25" t="s">
+      <c r="M46" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" ht="90" spans="1:13">
-      <c r="A47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C47" s="12" t="s">
+      <c r="A47" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D47" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E47" s="12" t="s">
+      <c r="G47" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>202</v>
       </c>
       <c r="J47" t="s">
         <v>32</v>
       </c>
-      <c r="K47" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L47" s="31">
+      <c r="K47" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L47" s="33">
         <v>44586</v>
       </c>
-      <c r="M47" s="25" t="s">
+      <c r="M47" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="48" ht="60" spans="1:13">
-      <c r="A48" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C48" s="12" t="s">
+      <c r="A48" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D48" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E48" s="12" t="s">
+      <c r="F48" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="G48" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="G48" s="12" t="s">
+      <c r="J48" t="s">
         <v>206</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L48" s="33">
+        <v>44586</v>
+      </c>
+      <c r="M48" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" ht="90" spans="1:13">
+      <c r="A49" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="K48" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L48" s="31">
-        <v>44586</v>
-      </c>
-      <c r="M48" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" ht="90" spans="1:13">
-      <c r="A49" s="17" t="s">
+      <c r="B49" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B49" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C49" s="12" t="s">
+      <c r="D49" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D49" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E49" s="12" t="s">
+      <c r="F49" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="G49" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>212</v>
       </c>
       <c r="J49" t="s">
         <v>32</v>
       </c>
-      <c r="K49" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L49" s="31">
+      <c r="K49" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L49" s="33">
         <v>44586</v>
       </c>
-      <c r="M49" s="25" t="s">
+      <c r="M49" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="50" ht="34" customHeight="1" spans="1:13">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+    </row>
+    <row r="51" s="16" customFormat="1" ht="90" spans="1:13">
+      <c r="A51" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-    </row>
-    <row r="51" s="4" customFormat="1" ht="90" spans="1:13">
-      <c r="A51" s="13" t="s">
+      <c r="B51" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="C51" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="D51" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="E51" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="D51" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="E51" s="23" t="s">
+      <c r="G51" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="G51" s="23" t="s">
+      <c r="H51" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="J51" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="K51" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L51" s="32">
+        <v>44586</v>
+      </c>
+      <c r="M51" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="J51" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L51" s="30">
+    </row>
+    <row r="52" s="19" customFormat="1" ht="90" spans="1:13">
+      <c r="A52" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="J52" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L52" s="33">
         <v>44586</v>
       </c>
-      <c r="M51" s="23" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="52" s="7" customFormat="1" ht="90" spans="1:13">
-      <c r="A52" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="C52" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="G52" s="26" t="s">
+      <c r="M52" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" ht="90" spans="1:13">
+      <c r="A53" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="J52" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K52" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L52" s="31">
-        <v>44586</v>
-      </c>
-      <c r="M52" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" ht="90" spans="1:13">
-      <c r="A53" s="17" t="s">
+      <c r="B53" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C53" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="B53" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="C53" s="25" t="s">
+      <c r="D53" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E53" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="D53" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="E53" s="24" t="s">
+      <c r="G53" s="29" t="s">
         <v>227</v>
-      </c>
-      <c r="G53" s="26" t="s">
-        <v>228</v>
       </c>
       <c r="J53" t="s">
         <v>32</v>
@@ -3604,32 +3794,31 @@
       <c r="K53" t="s">
         <v>7</v>
       </c>
-      <c r="L53" s="31">
+      <c r="L53" s="33">
         <v>44586</v>
       </c>
-      <c r="M53" s="7" t="s">
+      <c r="M53" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="54" ht="90" spans="1:13">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C54" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B54" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="C54" s="25" t="s">
+      <c r="D54" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E54" s="29" t="s">
         <v>230</v>
       </c>
-      <c r="D54" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="E54" s="24" t="s">
+      <c r="G54" s="29" t="s">
         <v>231</v>
-      </c>
-      <c r="F54"/>
-      <c r="G54" s="26" t="s">
-        <v>232</v>
       </c>
       <c r="J54" t="s">
         <v>32</v>
@@ -3637,10 +3826,10 @@
       <c r="K54" t="s">
         <v>7</v>
       </c>
-      <c r="L54" s="31">
+      <c r="L54" s="33">
         <v>44586</v>
       </c>
-      <c r="M54" s="7" t="s">
+      <c r="M54" s="19" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3658,4 +3847,286 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="10.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="61.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="20.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="39.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="10.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="13.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="13.5714285714286" customWidth="1"/>
+    <col min="10" max="10" width="9.28571428571429" customWidth="1"/>
+    <col min="11" max="11" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="29" customHeight="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" ht="141" customHeight="1" spans="1:11">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" ht="119" customHeight="1" spans="1:11">
+      <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>250</v>
+      </c>
+      <c r="J3" t="s">
+        <v>251</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" ht="75" spans="1:11">
+      <c r="A4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G4" t="s">
+        <v>257</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J4" t="s">
+        <v>251</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="60" spans="1:11">
+      <c r="A5" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="105" spans="1:11">
+      <c r="A6" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="90" spans="1:11">
+      <c r="A7" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>